<commit_message>
Update CBSC cs syllabus class 10.xlsx
</commit_message>
<xml_diff>
--- a/BusinessManagement/Content Collection/CBSC Syllabus CS Class 10/CBSC cs syllabus class 10.xlsx
+++ b/BusinessManagement/Content Collection/CBSC Syllabus CS Class 10/CBSC cs syllabus class 10.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="20115" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="60" windowWidth="20115" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Information sheet" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t xml:space="preserve">Syllabus </t>
   </si>
@@ -77,12 +77,24 @@
   <si>
     <t xml:space="preserve">Marks distribution </t>
   </si>
+  <si>
+    <t>Multiple assessment</t>
+  </si>
+  <si>
+    <t>Portfolio</t>
+  </si>
+  <si>
+    <t>Practical</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Internal assessment </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -104,6 +116,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -113,7 +133,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -182,11 +202,69 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -206,6 +284,19 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -509,7 +600,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:I469"/>
   <sheetViews>
-    <sheetView view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView view="pageLayout" topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="K57" sqref="K57:L58"/>
     </sheetView>
   </sheetViews>
@@ -5268,55 +5359,435 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="9" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="11"/>
+    </row>
+    <row r="3" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B4" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C4" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D4" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E4" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F4" s="15" t="s">
         <v>18</v>
       </c>
     </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="12"/>
+      <c r="B5" s="12"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="12"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="1"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="1"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="1"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="1"/>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="1"/>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="1"/>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="1"/>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="1"/>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="1"/>
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="1"/>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="1"/>
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+      <c r="F30" s="1"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="1"/>
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+      <c r="F31" s="1"/>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A2:F2"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <headerFooter>
+    <oddHeader xml:space="preserve">&amp;C
+</oddHeader>
+  </headerFooter>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C26"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.85546875" customWidth="1"/>
+    <col min="3" max="3" width="11.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="10"/>
+      <c r="C2" s="11"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="1"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="1"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="1"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="1"/>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="1"/>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="1"/>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="1"/>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A2:C2"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <headerFooter>
+    <oddHeader>&amp;C&amp;G</oddHeader>
+  </headerFooter>
+  <legacyDrawingHF r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>